<commit_message>
Final tamilnadu datascraping of website
</commit_message>
<xml_diff>
--- a/tamil_nadu_temples.xlsx
+++ b/tamil_nadu_temples.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tamil Nadu Temples" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Temples" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -55,13 +55,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,17 +425,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="80" customWidth="1" min="2" max="2"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -448,415 +441,187 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>Information</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>63 Best Pilgrimage Sites in Tamil Nadu | Temples in Tamilnadu (2025)</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>COVID-19 Travel Guidelines Travel Agents +91-7799591230 Tour Enquiry Sign up | Login Hello! My Bookings Login Logout New User? Sign-up Tours Domestic Tours Karnataka Tamilnadu Kerala Goa Andhra South India Maharashtra Gujarat Rajasthan Golden Triangle North India North East India International Sri Lanka Thailand Bali Dubai Singapore Maldives(Discontinued) All Domestic Tours All International Tours Offbeat Tours Domestic Cruise Tours Resorts Jungle Lodges by JLR Jungle Lodges by JLR Kabini River Lodge Bandipur Safari Lodge JLR Kings Sanctuary River Tern Lodge Kali Adventure Camp Hampi Heritage &amp; Wilderness Resort K Gudi Wilderness Camp Car Rentals Destinations Getaways Hotels Tools Tourist Places on Drive Driving Directions * Workation * Tour Plans Blog List Property * Offers * We Are Hiring! Interested in this tour? Request QuoteBook Now Get Advanced Tour Plan Need Help with This Tour? Contact Us GetawaysTamilnaduAll Pilgrimage Destinations 63 Best Pilgrimage Sites in Tamil Nadu Best Tourist PlacesTopHill StationsSacred Pilgrimage SitesFamous Heritage Sites List View Map View Filter by Category Beaches Historical / Heritage Hill Stations Pilgrimage Waterfalls Wildlife Adventure / Trekking Lakes / Backwaters Nature Museum / Gallery Cities Show All States Andhra Pradesh Delhi Haryana Himachal Pradesh Karnataka Kerala Maharashtra Rajasthan Tamil Nadu Telangana Uttarakhand Uttar Pradesh</t>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Meenakshi Amman Temple, Madurai</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Meenakshi Amman Temple, located in Madurai, is one of the famous Shiva temples in Tamil Nadu which was built during the Nayak rule. Also known as the Meenakshi-Sundareshwar Temple, it is dedicated to Goddess Parvati as Meenakshi and her consort Lord Shiva as Sundareshwar. This Shiva temple in Tamil Nadu holds great importance for both tourists and locals and is an integral part of South India's culture. All the important festivals of Tamil Nadu are celebrated here with great pomp and show, especially the Chithirai Festival. It signifies the celestial marriage of Meenakshi and Sundareswarar, drawing a massive crowd of devotees.</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>Madurai</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>Historical &amp; Heritage | Pilgrimage | City Situated on the banks of the River Vaigai, Madurai is the third-largest city in Tamilnadu and one of the most famous places of pilgrimage in India. The city is situated about 209 km from Coimbatore and 464 km from Chennai. Also referred to as Athens of the East, Madhurai is the oldest continually inhabited city in the Indian peninsula, with a history dating back to the Sangam period of the pre-Christian era. Madurai was the seat of power of the Pandyan Empire. Often considered the cultural capital of Tamilnadu, Madurai is one of the top places to visit in tamilnadu. The city is very well known for Madurai Meenakshi Temple, among the most visited temple in South India tour packages.Meenakshi Temple, also known as Madurai Meenakshi, is the biggest landmark of Madurai and is one of the largest temples in India. The temple has stunning architecture and a significant testimony for Vishwakarma Brahmins for their master architecture in sculpting this temple. Along with Meenakshi Temple, Thirumalai Nayak Mahal &amp; Koodal Alagar Temple are other important places to visit as part of Madurai tour packages. ... Overview Madurai Packages from ₹6000 Madurai Tourist Places</t>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Sri Laxmi Narayanan Golden Temple, Vellore</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Also known as the Sripuram Golden Temple, it is located at Vellore in Tamil Nadu and is a part of almost all the south India tour packages. The temple is dedicated to Laxmi, the Goddess of wealth and prosperity and entirely built with pure gold, making it famous as the Golden Temple. Its outstanding carving, sculptures, artwork, and exquisite lighting further give it a unique charm. One of its kinds in the world, this Golden Temple of Tamil Nadu is surrounded by water and offers a magnificent sight to behold during the night.</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Rameshwaram</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage Rameshwaram is one of the popular places of pilgrimage in Tamilnadu as well as in India. Situated at a distance of 562 km from Chennai, the town is home to the famous Rameshwaram Temple, among the must include places in Tamilnadu Tour Packages. Dedicated to Lord Shiva, Rameshwaram Temple is one of the Jyotirlinga temples in India, and is one of the top attractions you must visit as part of Rameshwaram tour packages. It is significant for Hindus as a pilgrimage to Banaras is incomplete without a Pilgrimage to Rameswaram. This is also the place where Rama worshipped Lord Shiva to cleanse away the sin of killing Ravana. Rameswaram along with Dwarka, Puri and Badrinath form the four Char Dhams. Sri Ramanathaswamy Temple, Agnitheertham, Gandamadana Parvatham, Dhanushkodi, Kothandaraswamy Temple and Erwadi are some of the most visited attractions of Rameshwaram. Sri Ramanatha Swamy Temple is renowned for its magnificent corridors and massive sculptured pillars. The third corridor of Ramanathaswamy temple is the longest one in the world. ... Overview Rameshwaram Packages from ₹6250 Rameshwaram Tourist Places</t>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bala Murugan Temple, Siruvapuri</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Tamil Nadu is home to several famous Murugan temples, and one of them is the Bala Murugan temple in Siruvapuri. Murugan is another name for Lord Karthikeya, son of Lord Shiva and Goddess Parvati. The temple is 500 years old and famous among devotees to fulfil their wishes. Owing to this, hundreds of devotees visit this Murugan temple in Tamil Nadu each day to worship Lord Karthikeya and wish upon it. Besides, the temple complex has a shrine dedicated to Lord Murugan and his consort Devi Valli as depicted in wedlock. It is visited by couples who wish to get married.</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Srirangam</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage | Historical &amp; Heritage Srirangam, the beautiful river island, is one of the prominent places of pilgrimage in South India, and among the must include places in Tamil Nadu tour packages. About 13 km from Trichy, and 136 km from Madurai, it holds great cultural and religious significance in South India.Nestled between the Kaveri River and Kollidam River, Srirangam is home to Sri Ranganatha Swamy Temple, the world's grandest operational Hindu shrine. Dedicated to Lord Vishnu, it is the foremost among the 108 Divya Desams of Lord Vishnu, and among the must-include places in Srirangam tour. Jambukeswarar temple, Uthamar Kovil, Uraiyur Vekkali Amman Temple, Samayapuram Mariamman Temple, Kumara Vayalur Temple, Gunaseelam Temple, Sri Vadivazhagiya Nambi Perumal Temple, and the Kaattu Azhagiya Singar Temple, etc. are some other tourist places in Srirangam. The Chithirai car festival, Vasantotsavam, Jyeshtaabhishekam, Pavitrotsavam, Vaikunta Ekadashi, and Teppostavam are the popular festivals celebrated in Srirangam, Srirangam can be visited as part of Trichy packages as well. ... Overview Srirangam Tourist Places</t>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Navapashanam Temple, Devipattinam</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Navagraha temples in Tamil Nadu are a set of nine temples, each of them dedicated to one of the nine planetary deities. One of these famous Navagraha temples is the Navapashanam Temple located in Devipattinam, Tamil Nadu. The significance of this temple centres on the fact that devotees can worship all the nine planetary deities at once. It is also a famous Hindu pilgrimage site along with the Ramanathaswamy Temple at Rameshwaram, and the Adi Jagannatha Perumal Temple at Thiruppullani. Devotees believe that the shrines of the planetary deities at this Navagraha temple in Tamil Nadu were built by Lord Ram, an avatar of Lord Vishnu.</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>Kanyakumari</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage | Beach | Nature &amp; Scenic Located at the southernmost tip of the Indian Peninsula, Kanyakumari is one of the famous pilgrimage places to visit as part of Tamilnadu tour. It is about 242 km from Madurai and 707 km from Chennai.A place of great natural beauty, Kanyakumari is one of the popular href='/tamilnadu/best-places-to-visit' target='_blank'&gt;Tamilnadu Tourist Places. Swami Vivekananda is said to have been lived here for a while and meditated. Situated at the confluence of the Bay of Bengal, the Arabian Sea, and the Indian Ocean, this is the only place in India where one can enjoy the unique spectacle of Sunset and Moonrise simultaneously on full moon days. One of the main attractions in Kanyakumari is the Kumariamman Temple. Thiruvalluvar Statue, Vivekananda Rock Memorial, Gandhi Memorial, Padmanabhapuram Palace, Suchindram, Pechiparai Reservoir, Vattakottai Fort, St Xavier's Church and Udayagiri Fort are some of the top places to visit as part of Kanyakumari tour packages. Kanyakumari is also known for its spectacular beaches. Thengapattinam Beach, Sanguthurai Beach, and Chothavilai Beach are the important beaches near Kanyakumari. ... Overview Kanyakumari Packages from ₹6250 Kanyakumari Tourist Places</t>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Kumbakonam Brahma Temple, Kumbakonam</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Kumbakonam Brahma Temple in Tamil Nadu is one of the famous pilgrimage sites for the Hindus that is located in Thanjavur district. The temple is primarily dedicated to Lord Vishnu as Vedanarayana Perumal. Its sanctum also has a deity of Brahma which is placed on the right side of Lord Vishnu's deity, along with Goddesses Saraswati and Gayatri. On the left side is Yoganarasimha with Bhoodevi and Sridevi. Since Lord Brahma is said to be cursed for not being worshipped, the Kumbakonam Brahma Temple in Tamil Nadu is one of the rare temples dedicated to him in India.</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>Chidambaram</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>Historical &amp; Heritage | Pilgrimage Chidambaram is a pilgrimage town in Tamil Nadu. Well known for Nataraja Temple, Chidambaram temple is one of the most celebrated shrines in South India and also one of the famous Tamilnadu places to visit. It is about 66 km from Pondicherry, and 217 km from Chennai.Also known as Thillai, the town is known for the Thillai Nataraja Temple which is dedicated to Lord Shiva. Built during the 11th century, Chidambaram Nataraja Temple has a great religious as well as historic and cultural significance. This is one of the Panchabhoota Stalas signifying the five elements of wind (Kalahasti), water (Tiruvanaikka), fire (Tiruvannamalai), earth (Kanchipuram) and space (Chidambaram). Thillai Kaali Amman Temple, Pichavaram, Sattanathar Temple, Bhuvanagiri, Parangipettai, Annamalai University, Kollidam (river) and Poompuhar are the other prominent places to visit as part of Chidambaram tour packages.Brahmotsavam, Ani Thirumanjanam, Thai Poosam and Arudra Dharshan are some of the Nataraja Temple festivals that attract large crowds from far and nearby places. Natyanjali Dance Festival is a major festival held in February. Many eminent dancers give their performances during this festival. ... Overview Chidambaram Packages from ₹7900 Chidambaram Tourist Places</t>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Brihadeeswarar Temple, Thanjavur</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Brihadeeswarar or Brihadisvara is yet another famous Shiva temple in Tamil Nadu. It was built during the Chola Dynasty in the 11 century AD. The temple is located in the Thanjavur district and enjoys the status of a UNESCO World Heritage Site as one of the Great Living Chola Temples in India. Besides its magnificent structure, the 216 feet tall Vimana, along with its 80 tonnes Kumban, stands in the temple complex and attracts tourists interested to learn about great architectural designs from Indian history. As one of the famous Shiva temples in Tamil Nadu, it is visited by thousands of devotees every day.</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>Kanchipuram</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>Historical &amp; Heritage | Pilgrimage Kanchipuram or Kanchi is one of the most famous places of pilgrimage in Tamilnadu. It is situated at a distance of 75 km from Chennai. Located on the bank of the Palar River, Kanchipuram is one of the oldest cities in India and was served as the capital of the Pallava Dynasty. Kanchipuram is one of the most popular places to visit near Chennai. Kanchi is known for its temples and silk sarees which are woven manually. Kamakshi Amman Temple is the landmark of Kanchipuram, and among the most popular places to visit in Kanchipuram. Varadharaja Perumal Temple, Kailasanathar Temple, Karchapeshwarar Temple, Sri Ekambarnathar Temple are the other prominent temples to visit as part of Kanchipuram tour packages. The temples of Kanchipuram are known for their grandeur and great architecture.Kanchipuram is a traditional center of silk weaving and handloom industries for producing Kanchipuram Sarees. In 2005, 'Kanchipuram Silk Sarees' received the Geographical Indication tag, the first product in India to carry this label. ... Overview Kanchipuram Packages from ₹1550 Kanchipuram Tourist Places</t>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Arulmigu Brahmapureeswarar Temple, Tirupattur</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>The mythological reference of this temple tells us the story of Lord Brahma's overwhelming pride which made him feel more powerful than Shiva. This sense of pride provoked Lord Shiva to destroy Lord Brahma's fifth head and curse him to lose all his powers. Realizing his mistake, Lord Brahma offered huge penance to Lord Shiva at various places. During his pilgrimage, he worshipped the Lord under a tree at the temple's site and took water for the rituals from the nearby tank, which was named Brahma Theertham. As Brahma worshipped Lord Shiva at this place, it is named Brahmapureeswarar.</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>Thanjavur</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>Historical &amp; Heritage | Pilgrimage Thanjavur, also known as Tanjore, is one of the popular places of href='/tamilnadu/heritage' target='_blank'&gt;heritage in Tamilnadu as it has a rich historical heritage and is a prism of ancient as well as the modern south Indian civilizations. It is situated about 170 km from Madurai, and 326 km from Chennai. Situated on the banks of River Cauvery, it is one of the top places to visit as part of Madurai tour packages. The city was once the stronghold of the historic Cholas. Since then, Thanjavur has been one of the chief political, cultural and religious centers of South India. Thanjavur is famous for the Brihadeeswarar Temple built by Rajaraja Chola in the year 1010 AD. Also known as the Big Temple, Brihadeeswarar Temple is one of UNESCO World Heritage Sites and among the most important heritage sites in India. The temple is considered to be one of the best specimens of South Indian temple architecture and among the must-visit places as part of Thanjavur tour packages.Apart from Brihadeeswarar Temple, Thanjavur and the surrounding areas have several important tourist attractions like Thanjavur Palace, Kumbakonam, Darasuram, Gangaikonda Cholapuram, Thiruvaiyaru, Thirubuvanam, etc. ... Overview Thanjavur Tourist Places</t>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Ekambareswarar Temple, Kanchipuram</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Tamil Nadu has many famous temples that are dedicated to Lord Shiva. One of them is the Ekambareswarar Temple, located in Kanchipuram. It is famous as one of the Pancha Bhoota Sthalas and signifies the element Earth. Devotees visit the temple to worship Lord Shiva, as Ekambareswarar or Ekambaranathar, in the form of a Lingam and an idol Prithvi Lingam. Legend has it that Goddess Parvati used to worship Lord Shiva in the form of Prithvi Lingam (Shiva Lingam made of sand) at this place, under a mango tree. The lord, impressed by this gesture, materialized in person and married the Goddess.</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>Tiruvannamalai</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage The sacred site of Tiruvannamalai is one of the prominent places of pilgrimages in Tamilnadu, and among the best places to visit near Chennai. Situated at 115 km Pondicherry, 191 km from Trichy, and 196 km from Chennai, Thiruvannamalai is known as one of the major pilgrimage centres of India.Tiruvannamalai is known for Annamalaiyar Temple, one of the Pancha Bhoota Stalas of Lord Shiva, representing the 5 elements of nature. Legend has it that Shiva appeared as a massive column of fire in this temple. This temple features one of the tallest temple towers in India and is visited as part of Tiruvannamalai packages. Sri Ramana Ashram, Sathanur Dam, Sri Seshadri Swamigal Ashram, Virupaksha Cave, Mamara Cave, Skandashramam, and Annamalaiyar Temple View Point are some of the top places to visit in Tiruvannamalai.Thiruvannamalai boasts a vibrant culture centered on the renowned Annamalaiyar Temple. Visitors can also explore nearby sites such as Tirumalai Jain Temples, Gingee Fort, and Padaveedu. Thiruvannamalai temple darshan usually takes 2-3 hours but can take upto 5-6 hours on festival dates and holidays. ... Overview Tiruvannamalai Tourist Places</t>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Ramanathaswamy Temple, Rameshwaram</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Ramanathaswamy Temple in Rameshwaram is one of the 12 Jyotirlinga temples and a holy pilgrimage site for the Hindus. It is believed that the Shiva Lingam placed at the temple was built and worshipped by Lord Ram before crossing the bridge to Lanka, and that is where the name Ramanathaswamy was derived. Lord Ram wanted to seek forgiveness from his lord for the sins he would commit during the war against Ravana. He requested Hanuman to bring a Lingam from the Himalayas. However, with his delayed arrival, Lord Ram decided to build a Lingam from sand, which is placed at the sanctum. The temple has another lingam which was brought from Kailash and is called Vishwalingam.</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>Kumbakonam</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage Kumbakonam is an ancient temple town located amidst the two rivers Cauvery and Arasalar in the Thanjavur district of Tamil Nadu. About 235 km from Madurai, and 282 km from Chennai, it is one of the famous places of pilgrimage in Tamilnadu, and among the popular places to visit near Chennai. Kumbakonam is known for its temples and mutts (monasteries). There are around 188 Hindu temples within the municipal limits of Kumbakonam. Adi Kumbeswarar Temple, Nageswaraswamy temple and Kasi Viswanathar temple are the prominent temples to visit as part of Kumbakonam tour packages. Sarangapani temple is the largest Vaishnava shrine present in Kumbakonam. Patteeswaram, the Oppiliappan Kovil, the Swamimalai Murugan temple and the Airavateeswarar Temple are the other temples located in the vicinity of Kumbakonam.The town is well - known for its prestigious educational institutions and carved Panchaloha idols, silk products, brass, and metal wares. The important festival of Kumbakonam is the Mahamaham festival. It takes place once in 12 years during the Tamil Month of Masi (February/March) and lakhs of pilgrims visit Kumbakonam and takes a holy bath in the sacred Mahamaham Tank. ... Overview Kumbakonam Tourist Places</t>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Kapaleeshwarar Temple, Chennai</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>This temple is located in Mylapore, a district of Chennai in Tamil Nadu. It was built in the 7th century CE under the reign of Pallava King. However, the original structure was destroyed by the Portuguese, and the Kapaleeshwarar Temple structure that stands today was restored by the Vijayanagara Kings in the 16th century. Dedicated to Lord Shiva, the temple is among the famous pilgrimage sites that attract devotees from all over the country. Legends say that Goddess Parvati, as Mayil, performed a huge penance for Lord Shiva at the site. The temple complex has a small shrine of the Goddess in the form of a peahen placed under the Punnai tree and depicts her story.</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>Tirunelveli</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage Tirunelveli is a city situated on the banks of the river Thamirabarani in Tamilnadu. About 158 km from Madurai, 291 km from Trichy, and 623 km from Chennai, Tirunelveli is the most popular places to visit near Trichy, and among the must include places in Tamilnadu packages.Also known as Nellai, Tirunelveli is positioned close to the southern tip of India and is very eminent for various geographical features. Tirunelveli has a rich cultural and architectural heritage which is evident from the various temples, and churches located here, and are the must include places in Tirunelveli packages. Nellaiappar Temple, Venkatachalapathy Temple, Sankaranainar Kovil, Allagammai Kashi Vishvanathar, Holy Trinity Cathedral, the Mela Tiruvenkatanathapuram Temple, and Mundanthurai-Kalakad Wildlife are some of the top tourist places in Tirunelveli. The city is also famous for Tirunelveli Halwa and also known as Halwa city and Oxford of South India. The annual Car Festival of Nellaiappar Temple is the major festival celebrated at Tirunelveli. ... Overview Tirunelveli Packages from ₹5250 Tirunelveli Tourist Places</t>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Elk Hill Murugan Temple, Ooty</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Besides being one of the popular hill stations in Tamil Nadu, Ooty is home to the Elk Hill Murugan Temple, dedicated to Lord Murugan. This famous Murugan temple in Tamil Nadu catches your eye for its similarity to the Batu Caves in Malaysia. The temple is perched atop a small hill named Elk Hill and surrounded by a serene atmosphere with picturesque views. Along with the presiding 40 feet deity of Lord Murugan that resembles the deity at Batu Caves, the temple also houses the deities of Lord Ganesha, Lord Shiva, and Goddess Shakti, also known as Kali.</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t>Tenkasi</t>
-        </is>
-      </c>
-      <c r="B13" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage Tenkasi is the second largest town in the Tirunelveli district of Tamil Nadu. Situated on the Madurai - Kollam highway, it is one of the popular places to visit near Trivandrum, and among the top Tamilnadu places to visit. It is situated about 109 km from Trivandrum, 132 km from Kanyakumari, and 160 km from Madurai.Tenkasi is famous for numerous waterfalls spread around the region including the famous Courtallam Falls, among the must include places in Tenkasi packages. River Chittar flows through this picturesque destination favoured amongst tourists.The Word Tenkasi means Kasi of the South referring to the Kasiviswanathar temple situated in the town. Kulasekaranathar Temple, Kannimaramman Temple, Anggalap Parameshwari Temple, and Esakki Amman Kovil are the other prominent Tenkasi tourist places. ... Overview Tenkasi Packages from ₹5250 Tenkasi Tourist Places</t>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Kumari Amman Temple, Kanyakumari</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Dedicated to the virgin Goddess Kanya Kumari, an avatar of Goddess Shakti, the temple dates back to 3000 years. Its complex has a deity in the form of a beautiful girl holding a string of beads in her right hand. Mythological beliefs state that Goddess Shakti took this avatar upon being requested by the Devtas to save them from the Demon King Banasura. As he was blessed by Lord Shiva for only being vanquished by a virgin girl, the Goddess took this avatar to defeat him. However, enchanted by her beauty, the Banasura tried to force her into a marriage that eventually became the cause of his death.</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>Sri Sankaranarayana Swamy Temple - Sankarankovil</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 16 km from Thirumalpuram and 56 km from Tirunelveli, Sri Sankaranarayana Swamy Temple is a famous Hindu temple situated at Sankarankovil in Tirunelveli district of Tamilnadu. It is one of the top pilgrimage places to visit in Tirunelveli region and also one of the popular temples in Tamilnadu.The temple is dedicated to Sankaranarayanar, who is the combined manifestation of Shiva and Vishnu. This temple was built by Ukkira Pandiya Thevar in the 11th century AD. This temple also called as Avudaiamman Kovil or Davasu Kovil. According to mythology, once the devotees of Lord Vishnu and Lord Shiva quarreled with each other to determine whose god is powerful. Then Lord Shiva appeared as Sankaranarayanar to mark his devotees to understand that both Hari and Shiva are one and the same. So it is held sacred by Saivites and Vaishnavites as well. Hence this temple depicts the concept of Hari and Haran being one God.The temple of Sankaranarayana is situated on 4.5 acre site in the heart of the Sankarankovil Town. It is one of the Pancha Bootha Sthalas in the South Pandiya country. With an imposing Rajagopuram, rising to a height of 135 feet with nine tiers, this temple is surrounded by high walls and the tower has many beautiful images. Lord Sri Sankaranarayana is the main deity in this temple. The right portion of the idol has sandal and indicates Lord Siva, with cobra around his neck &amp; moon above his head. The left side of the idol indicates Lord Vishnu ... ... Overview Sri Sankaranarayana Swamy Temple - Sankarankovil Tourist Places</t>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Nagaraja Temple, Nagercoil</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Nagercoil is a beautiful town that offers peaceful and serene sightseeing places in Tamil Nadu. However, what attracts devotees to this town is its famous Nagaraja Temple. Located in Nagercoil, the temple is dedicated to the King of Serpents - Nagaraja. The inscriptions and literary evidence present at the temple complex indicate being worshipped by both Jains and Hindus. The original temple built in the pre 12th century only had the Jain iconography of the Tirthankaras and Padmavati Devi. New Hindu shrines were added to its complex in the 17th century. Since then, the iconographies of both religions have been a part of the temple's sanctum.</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>Devipattinam Navagraha Temple</t>
-        </is>
-      </c>
-      <c r="B15" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 15 km from Ramanathapuram, and 65 km from Rameshwaram, Devipattinam is a beautiful coastal village situated in the Ramanathapuram district of Tamilnadu. It is one of the popular Rameshwaram places to visit. Devipatnam, along with Rameshwaram and Thiruppullani are associated with the Hindu sacred epic Ramayana. Also known as Navapashanam, this holy town is famous for the Navagraha Temple. According to the legend, Lord Rama when going to war to kill Ravana had worshipped navagrahas by installing nine different stones, each symbolizing the nine celestial bodies to calmed the sea. It is said that since then, 9 navagraha stones are located in the sea, at a distance of about 100 meters from the seashore. These can be seen in the morning when the level of seawater is low; however in the evenings when the tides are high, most of the navagraha stones are submerged in the water.This small village also has a temple dedicated to Devi. It is said to be the place where Mahishasura was killed by Goddess Durga Devi. There are two other temples here, one dedicated to Thilakesava and the other to Jagannatha. The Thilakeshwar Temple is dedicated to Shiva and Parvathi (Durga). Shiva here is known as Thilakeswarar and the Goddess is known as Soundaryanayaki. Devotees at the temple offer nine varieties of grains to the Gods and Goddesses. The beach is full of multicolored shells and corals ... ... Overview Devipattinam Navagraha Temple Tourist Places</t>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Thillai Nataraja Temple, Chidambaram</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>As the name says, the temple is dedicated to the Nataraja avatar of Lord Shiva, a divine dancer. It is among the famous ancient temples in Tamil Nadu known for their religious and architectural significance. People believe that this temple is located at the centre of Earth's magnetic field. Its sanctum is named Chitsabha and houses the deities of Natraja and his consort Sivakamasundri. The temple was built in the 11th century during the Pallava rule. It is one of the Pancha Bhoota Sthalas dedicated to the five elements of the universe, namely Earth, Air, Fire, Water, and Space, and signifies the element Space.</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>Papanasam Temple</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 15 km from Ambasamudram and 47 km from Tirunelveli, Papanasam is a small town in Ambasamudram Taluk of Tirunelveli district in Tamilnadu. It is one of the popular picnic spots in Tirunelveli.Papanasam has a famous temple called the Papanasam Sivan Temple which lies on the banks of Thamirabarani River. Constructed in the Dravidian style of architecture, the holy shrine is dedicated to Lord Shiva and his consort Parvati who are worshipped as Papanasanathar and Ulagammai respectively. This is the place where Saint Agasthiyar got the Kalyana dharshan of Lord Shiva and Parvati along with his wife Lopamudra. The Shiva lingam of the temple is completely made up of Rudraksha. Of the nine Kailash Kshetras - Nava Kailash, Papanasam is the first place and is attributed to Sun God. Hence, the place is known as Surya Kshetra and Surya Kailash. Devotees strongly believe that Lord Shiva in this temple is most powerful and cures all kind of diseases. The temple is famous for its Chittirai Peruvila where the festivities used to happen for 13 days. Another attraction of this village is the Papanasam Dam, also known as the Thamirabarani River Dam. It is believed to have been built during the British era and is surrounded by high mountains and huge trees. The dam is about 240 m high, 5.4 m wide and 265 m long and has a total catchment area of around 147 sq. km. Boating is possible in the lake but swimming is strictly prohibited as it is populated with crocodiles. ... ... Overview</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="inlineStr">
-        <is>
-          <t>Thirupullani</t>
-        </is>
-      </c>
-      <c r="B17" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 15 km from Ramanathapuram, and 66 km from Rameshwaram, Thirupullani is a temple town situated near Rameshwaram. It is one of the prominent places of pilgrimage in Tamilnadu, and among the must-visit places during your Rameshwaram Trip.The town is known for Aadi Jagannatha Perumal Temple dedicated to Lord Vishnu. Popularly known as Thirupullani Temple, it is one of the 108 Divya Desam temples of Lord Vishnu. It is also known as Dharbasayanam as Rama took rest on a couch of grass at this place. Other names of this place are Thiruvadanai, Pularanyam, Adhisethu and Ratnaharam. This ancient temple not only attracts visitors because of its sacredness but also for its historical background and architectural excellence. Built during the reign of Cholas, various contributions were made to this temple during Pandyan rule and the rule of Sethupathy Kings. It is now maintained by the Hindu Religious and Endowment Board of Tamil Nadu Government.Built-in the Dravidian style of architecture, the presiding deity of the temple is Lord Dharba Sayana Rama. The specialty of this temple is that Lord has been shown in a reclining posture. There are also separate shrines for Goddess Padmasini, who is the consort of Lord Adi Jagannatha, Goddess Shridevi, Goddess Bhudevi, Lord Krishna. Timings: 7 AM - 12.30 PM &amp; 3.30 PM - 8.30 PM ... Overview Thirupullani Tourist Places</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>Mangalanatha Swamy Temple - Uthirakosamangai</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 70 km from Rameshwaram and 15 km from Ramanathapuram. Uthirakosamangai is famous for an ancient Siva temple considered to be 3000 years old. This is the place where Siva transferred the secrets of Vedas to Parvati. Uthiram means (updesham) kosam (secrets) Parvati (Mangai) hence this place is known as Uthira Kosa Mangai.The main deity here is Mangalanathar (Siva) and his consort is Mangleshwari. The main attraction of this temple is a statue of Natarajar made of emerlad which is about 51/2 feet tall. This idol is known as Margatha Natarajar and the deity is always covered with sandal paste. Only in the Tamil month of Margazhi on Tiruvathira nakshtram the sandal paste gets removed and there is abhishekam for the idol and this special darshan is known as Arudhra darishanam.There is a Nandi just outside the sanctum and a bigger Nandi in the outer prakaram known here as Pradosha Nandi. Special poojas are conducted here on Pradosham days in the evenings as it is believed that Siva dances between the horns of Nandi during that time.Annual 'Arudhra' festival in December attracts a large number of devotees on this day and on the next day again the idol gets smeared with sandal paste. ... Overview Mangalanatha Swamy Temple - Uthirakosamangai Tourist Places</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t>Anubhavi Subramaniar Temple</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 19 km from Coimbatore, Sri Anubhavi Subramaniar Temple also known as Anuvavi Subramaniar Temple is a Hindu temple located at Anuvavi Hills in Periya Thadagam in the outskirts of Coimbatore. It is one of the ancient temples in Coimbatore, and among the must-visit places as part of Coimbatore Tour Packages.Located on the Anaikatty highway, Sri Anuvavi Subramaniar Temple is dedicated to Lord Murugan and is one of the religious shrines in the region. In earlier days, this place was actually called Hanu Bhavi where the word Hanu stands for Sri Anjaneya, and Vavi means Water Source in Tamil. As per the mythology, Sri Anjaneyar felt thirsty while passing through this hill with the Sanjeevi mount. He prayed to Lord Muruga here for water. Lord punched a place here with His Vel from where water sprang up and flowed like a river. Till now, the origin of the spring in the temple could not be discovered. As Kumara-Muruga helped Hanuman, the hill is also praised as Hanumakumaran Malai. It is believed that the sanctum sanctorum of the temple was built by Karikala Chola in the early Christian Era. The Ardha Mandapa and Mahamandapa were built during the Kongu Chola Period (11th to 13th centuries). From 14th to 17th centuries, the Hoysala, Vijayanagar, and Nayaka kings gave endowments. The famous Kanaka Sabhai was built by Alagadri Nayak of Madurai in the 17th century. Tippu Sultan of Mysore attached half of ... ... Overview Anubhavi Subramaniar Temple Tourist Places</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="inlineStr">
-        <is>
-          <t>Eachanari Vinayagar Temple</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 15 km from Coimbatore, Arulmigu Eachanari Vinayagar Temple is a Hindu temple located at Eachanari near Coimbatore, Tamil Nadu, India. Situated on Coimbatore - Pollachi Main Road, it is one of the prominent temples in Coimbatore, and among the must-visit places during your Coimbatore Tour.Eachanari Vinayagar Temple is dedicated to elephant god Ganesha. There is an interesting little legend to this temple. It is said that when the idol of Lord Vinayagar was being transported from Madurai in a cart for installation at Perur Pateeswarar Temple, the axle of the cart broke. When the devotees tried to move the idol, the efforts did not materialize and this is how this temple came into being. The construction of the temple was done around 16 century AD, and it has been an important religious center ever since.The temple follows typical Dravidian-style architecture. The temple tower rises in layers, with many Hindu gods and goddesses and sacred animals and other motifs inscribed on it. The main deity's idol is about 6 feet in height and is 3 feet in diameter. The deity's face is black with a tilak on the forehead - typical to idols in the South Indian temple. The body of the deity was plated with bright gold in 2004.The main attraction of the Eachanari Vinayagar Temple is the daily Ganapathi Homam held everyday early morning at 5.30 PM, and is a costly affair, to both perform the offerings as ... ... Overview Eachanari Vinayagar Temple Tourist Places</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="inlineStr">
-        <is>
-          <t>Thirumoorthy Hills &amp; Waterfall</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage | Waterfall | Lake &amp; Backwater At a distance of 38 km from Pollachi, Thirumoorthy Hills is one of the charming outdoors near Pollachi. A part of the Anamalai range of the Western Ghats, it is one of the famous places to visit in near Pollachi.At the foot of the hills is the Thirumoorthy Temple, also known as Sri Amanalingeswarar Temple. A perennial stream flows by the side of the temple. The temple is dedicated to the Hindu trinity, Lord Shiva, Lord Vishnu, and Lord Brahma. Legend says that Athri Maharishi and his wife Anasuya Devi resided in these hills, and the Gods of the Hindu trinity had come down to test their devotion. The Gods asked Anasuya Devi to make their offerings in nudity. She agreed and changed the Gods as babies with her devotion, fed them &amp; put them to sleep in a cradle. Athri came back afterward and hearing the story from Anasuya praised the three gods sleeping in the cradle. Later, the Trinities come back to their original form and give a boon to Anasuya. According to her wish, three children were born to her - Shiva is born as Sage Durvasa, Vishnu as Dattatreya, and Brahma as Chandra (Moon). Hence, this region is named as Thirumoorthy Hills.Thirumoorthy Dam has been constructed adjoining the Thirumurthy Hill near Amanalingeswarar Temple. The panorama of the Anamalai Hills surrounding the shimmering blue waters of the reservoir is a sight to behold. This area is a popular spot for shooting films thanks to the beauty of the region. It is the perfect place for tourists who love ... ... Overview Thirumoorthy Hills &amp; Waterfall Tourist Places</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Adikesava Perumal Temple - Thiruvattaru</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 7 km from Marthandam and 45 km from Kanyakumari, Sri Adikesava Perumal Temple is a Hindu temple located in Thiruvattaru. It is one of the 108 divya desams of Sri Vaishnavas and also one of the popular places of pilgrimage in Kanyakumari. The temple is dedicated to Sri Adikesava Perumal, meaning 'Foremost Friend'. According to the legend, Lord Adikesava defeated the demon Kesi. The demon's wife prayed to the River Ganges and River Thamirabarani and created destruction. They came in spate to wash off the Lord. Mother Earth simply raised the ground level where Perumal was reclining. Both Rivers went round the Lord, prayed to Him and continued to flow round as two garlands. Thus, the formation of the rivers made in a circle came to be known as Thiruvattaru.The temple was built in Dravidian style architecture with wooden pillars, doors and roofs. The presiding deity here is in reclining posture along with Goddess Maragathavalli Nachiar. Though there are similarities between the Anantha Padmanabhaswamy Temple of Thiruvananthapuram, the Thiruvattar temple is older. The gigantic idol of the Lord stands at 22 feet, bigger than Anantha Padmanabhaswamy. The presiding deity is made of mustard, lime powder and jaggery. The lord is lying on his snake couch and has to be viewed through three doors. Adikesava Perumal's feet is on the left and head on the right; it is the reverse in Anantha Padmanabhaswamy Temple. A Shiva lingam is situated near Lord Adikesava ... ... Overview Adikesava Perumal Temple - Thiruvattaru Tourist Places</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="2" t="inlineStr">
-        <is>
-          <t>Samanar Hills</t>
-        </is>
-      </c>
-      <c r="B23" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 10 km from Madurai Junction Railway Station, Samanar Hills is a rocky stretch of hills located near Keelakuyilkudi village in the Madurai District of Tamil Nadu, India. Also known as Samanar Malai or Amanarmalai or Melmalai, it is one of the prominent places to visit as part of Madurai heritage packages.Situated at the intersection of NH-44 and NH-85, the Samanar Hills, characterized by their rocky terrain, begin near the village of Keelakuyilkudi and extend eastward towards southern Madurai. These hillocks are significant for housing numerous Jain and Hindu monuments. The Archaeological Survey of India has designated the Samanar Hills as a protected site. The name 'Samanar' translates to Jain in Tamil, while 'malai' means hill.The Samanar Hills feature a range of monuments that date from the 2nd century BC to the 12th century CE. Among these, two notable collections of Jain monuments stand out - Settipodavu site &amp; Pechchipallam site. The Settipodavu site, located at the southwestern slope, includes a Jain cave from the 10th century, which is accessible via a short ascent from the base. This site has an image of Lord Mahavira, the last Tirthankara of Jainism, along with flat stones that served as resting places for Jain monks.On the southeastern slope, at a higher elevation, lies the Pechchipallam site, which contains eight Jain sculptures, including those of Bahubali, Mahavir, ... ... Overview Samanar Hills Tourist Places</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="2" t="inlineStr">
-        <is>
-          <t>Sivasailam Temple</t>
-        </is>
-      </c>
-      <c r="B24" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 12 km from Papanasam and 47 km from Tirunelveli, Sri Sivasailanathar Paramakalyani Temple is a 500 year old Saivaite temple situated on the banks of River Gadana at Sivasailam in Tamilnadu. Popularly called as Sivasailam Temple, this is one of the famous Shiva temples near Tirunelveli. The Sivasailam Temple is dedicated to Lord Sivasailanathar and Goddess Parvati. Built by Pandiyas, the temple is surrounded by Velli malai, Mulli malai and Podhigai hills. It is believed that the Shiva Lingam in the sanctum is swayambhu lingam. At the back of the statue, there are lines that appear like hair, so he is also called Sadaiappar. This can be seen through a hole while strolling around the sanctum sanctorum. This is visible only when the Archakar gives Aarathi at the back of the lingam. The temple is huge with many mandapams and carved pillars. The principle gopuram has five stories and is embellished with numerous statues. The specialty of the temple is the huge statue of Nandi. Legend says that the Nandi was sculpted so beautifully that if came to life and started to lift off. Hence, the sculptor had to stroke it on its back so that it remained seated. The mark of the stroke can be seen today. Besides Lord Shiva, Vinayakar, Murugan, 63 Nyanmars, Dakshina Moorthy, and Natarjar are the other deities in this temple. There is a separate shrine for Goddess Paramakalyani which is situated next to the main sanctum. There are also some stone inscriptions ... ... Overview</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="2" t="inlineStr">
-        <is>
-          <t>Idaikattur Church / Sacred Heart Shrine</t>
-        </is>
-      </c>
-      <c r="B25" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 41 km from Madurai, the Sacred Heart Shrine is a Catholic church in Idaikattur in Tamil Nadu. It is one of the famous churches in Tamil Nadu, and among the top places to visit near Madurai. The Sacred Heart Shrine, commonly known as Idaikattur Church, was established in 1894 by French missionary Father Ferdinand Celle, following the guidance of a French Anglican woman named May Anne. She had been afflicted by a severe illness which doctors weren't able to cure. According to the narrative, she devoted nine consecutive days to prayer for the Sacred Heart of Jesus and subsequently experienced a complete recovery. In gratitude for this miracle, she contributed 2,000 francs towards the construction of the Sacred Heart Church in Idaikattur. The church underwent further expansion during the period of British rule.The church's architecture is remarkably captivating, attracting numerous tourists to the serene village of Idaikattur. It is recognized as a replica of the Reims Cathedral in France, yet it distinctly incorporates Indian architectural elements. Designed in the Gothic style, the church features a vaulted ceiling supported by columns with cantilever beams. These columns are linked to a circular terracotta ring adorned with garlands, flowers, and beads. The structure is composed of approximately 200 different types of tiles and molded bricks.The main altar stands out as the ... ... Overview Idaikattur Church / Sacred Heart Shrine Tourist Places</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="inlineStr">
-        <is>
-          <t>Narubunatha Swamy Temple</t>
-        </is>
-      </c>
-      <c r="B26" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 16 km from Ambasamudram and 30 km from Tirunelveli, Narubunatha Swamy Temple is an ancient Hindu temple situated at Thirupudaimaruthur near Veeravanallur in Ambasamudram Taluk of Tirunelveli district, Tamilnadu. Situated at the merging place of Gadana River &amp; Thamirabarani River, this temple is one of the oldest temples in Tirunelveli region.Also known as Thirupudaimaruthur Temple, the temple is dedicated to Lord Shiva and is more than 1200 years old. Maravarman, the king of Madurai and his son had built a small temple in 650 BCE. After that, Pandiyas, Vijayanagara Kings and Kalakkad Kings expanded the temple. The sanctum sanctorum has a huge Shiva lingam, which is known as Pudaar Jeeneshwarar or Narumbunathar. The Shiva lingam leans slightly towards the left side and has marks of scratches made by deer and sickle cut. According to the legend, the region was under the rule of Maravarman then. He came to this place dense with Marudha trees for hunting. He targeted a deer which hid itself in the hole of a tree. The king ordered to cut the tree to get the deer out. But blood came out of the tree where the king found a Shiva lingam with a hit on the head caused by the instrument. He heard a voice saying that Shiva himself graced them through the deer. He built the temple as directed by the Lord. Situated in 6 acres of land, Thirupudaimaruthur Temple's compound walls measure 575 feet in length. The temple gopuram has five tiers. There are many ... ... Overview Narubunatha Swamy Temple Tourist Places</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="2" t="inlineStr">
-        <is>
-          <t>Thirumohoor Kalamegaperumal Temple</t>
-        </is>
-      </c>
-      <c r="B27" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 20 km from Madurai, ISKCON Temple Madurai is a revered Hindu temple situated in the Mani Nagaram Main Road in Madurai. It is one of the revered Pigrimage sites near Madurai. The Thirumohoor Kalamegaperumal Temple, also referred to as Thirumohoor or Tirumogoor Temple, is a significant Hindu temple dedicated to Lord Vishnu. It is recognized as one of the 108 Divya Desams, where Vishnu is revered as Kalamega Perumal, alongside his consort Lakshmi, known as Mohanavalli Thayar. The temple has a rich history and was originally constructed during the reign of Pandyan King Sadaiya Varman Sundara Pandiyan. The current structure, which features various enhancements, was established during the era of the Madurai Nayaks. Inscriptions within the temple provide insights into its construction and history. The temple is currently overseen by the Hindu Religious and Endowment Board of the Tamil Nadu Government.According to Hindu mythology, the presiding deity is said to have manifested as the enchanting Mohini to entice the asuras to aid devas during the Samudra Manthanam. The temple is also referred to as Mohanapuram and Mohanakshetram. Numerous esteemed poets and saints, including Manavala Mamunigal, Thirumangai Azhwar, Nammazhwar, Pillai Perumal Iyengar, Kalamega Pulavar, and Thiruninravur Tirumalai, have composed verses in praise of this temple. Additionally, Thirumohoor is mentioned in revered ... ... Overview Thirumohoor Kalamegaperumal Temple Tourist Places</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="2" t="inlineStr">
-        <is>
-          <t>Thirukkurungudi</t>
-        </is>
-      </c>
-      <c r="B28" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 45 km from Nagercoil, 46 km from Tirunelveli and 49 km from Kanyakumari, Thirukkurungudi is a holy place for Hindus situated on the banks of Nambi River at the foot hills of Mahendragiri in Tamilnadu.There are five Nambis in this Kshetram. They are Ninra Nambi (Standing posture), Irundha Nambi (Sitting posture), Kidandha Nambi (Sleeping posture), Thiruparkadal Nambi and Thirumalai Nambi. Of these, Ninra Nambi Temple is the main temple and is located in the center of the town flanked by four big Mada Veethis. The Nambi Rayar Temple or Thirukkurungudi Temple is 1300 years old. It is also called as Vaamana Kshetram and is one among the 108 divya desams of Lord Vishnu. According to the legend, Goddess Bhudevi was abducted by the demon Hiranyaksha and hid her deep under the ocean. All the deities and sages prayed to Lord Vishnu to retrieve Mother Earth from the demon. Lord Vishnu transformed into a wild boar and plunged into deep under the ocean. Lord Varaha had fierce battle with Hiranyaksha and saved Mother Earth. After this glorious incident Lord Vishnu along with Goddess Bhudevi arrived on this sacred land. He passionately looked upon Goddess and shrunk his terrifying size into normal. Thus, this place has got in its name 'Thirukkurungudi'.Covering an area of 18 acres, the temple has five prakarams, and is surrounded by a massive wall, crowned with a five tiered gopuram. The Vijayanagara rulers and the Nayaks of Madurai have made several ... ... Overview Thirukkurungudi Tourist Places</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="2" t="inlineStr">
-        <is>
-          <t>Sorimuthu Ayyanar Temple</t>
-        </is>
-      </c>
-      <c r="B29" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 12 km from Papanasam and 61 km from Tirunelveli, Arulmigu Sorimuthu Ayyanar Temple is situated between Papanasam and Karaiyar Dam in Tirunelveli district of Tamilnadu. Located on the bank of River Thamirabarani, this is one of the 6 important Sastha Temples in South India. The presiding deity of the temple is Mahalinga Swamy. Lord Dharma Sastha appears with his left leg bent and the right hanging down. Sorimuthu Ayyanar is a kuladevata for many families in the area. Families that are not aware of their kuladevata are also welcome here. As it is the first Ayyappan temple, people who resolve to begin the Sabarimala yatra, come here to wear their mala. The name of the temple is derived from 'Pon Soriyum Muthiar', which means the Lord who pours down golden rain on the plateau.Here, Muthianar is worshipped along with his two consorts - Pushkala and Poorna. Ayyappa's lieutenants, Sangili Bhootham, Thoosi Madan, Thulasi Madan, Pechi, Isakki and Pattavarayan are also worshipped here. There are also shrines dedicated to Vinayaka, Bhairava and Devi. Interestingly, this temple has many unique offerings. Here, devotees offer wooden legs and cloth dolls to the deity with humble prayers. People who suffer from leg and joint ailments offer wooden legs. Couples without children come here to pray for progeny by presenting rag dolls to express their desire. People offer bronze bells to Bhoothanathar and chappals to Valai Pagadai. Ashada Amavasya is celebrated ... ... Overview Sorimuthu Ayyanar Temple Tourist Places</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="2" t="inlineStr">
-        <is>
-          <t>Sri Vaikuntanatha Perumal Temple - Srivaikuntam</t>
-        </is>
-      </c>
-      <c r="B30" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 29 km from Tirunelveli and 39 km from Thoothukudi, Sri Vaikuntanatha Perumal Temple is an ancient temple situated at Srivaikuntam in Thoothukudi district of Tamilnadu. Located on the banks of the river Thamirabarani, this is one of the 108 divya desams of Lord Vishnu and the first of the Navatirupathis. Also called Srivaikuntam Temple and Kallapiran Temple, Sri Vaikuntanatha Perumal Temple is dedicated to Lord Vishnu in the form of Vaikuntanathar. It is believed that this temple was used as a fort in the fight between the legendary freedom fighter Veerapandiya Kattabomman and the British in the 1800s. The temple is classified as a Navatirupathi, the nine temples revered by Nammazhwar located on the banks of Thamirabarani River. This is the first in the series of these nine Tirupathi Temples.There are many legends associated with this temple. According to one legend, Somuka, a demon stole the four Vedas from Lord Brahma. Brahma was helpless and he did severe penance on the banks of Thamirabarani River seeking favour from Lord Vishnu. Pleased with the penance of Brahma, Vishnu agreed to help Brahma. Vishnu killed the demon and restored the Vedas to Brahma. Lord Vishnu set his abode as Srivaikuntam and resided there as Vaikuntanathar. Another story goes that the Lord, disguised as the thief, presented himself before the King to save the thief Kaaladhushakan, an ardent devotee of Lord Vishnu. Hence, the Lord here is also known as 'Kallapiran'. The ... ... Overview Sri Vaikuntanatha Perumal Temple - Srivaikuntam Tourist Places</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="2" t="inlineStr">
-        <is>
-          <t>Sri Kailasanathar Temple - Srivaikuntam</t>
-        </is>
-      </c>
-      <c r="B31" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 1 km from Sri Vaikuntanatha Swamy Temple, 30 km from Tirunelveli and 39 km from Thoothukudi, Sri Kailasanathar Temple is another important Hindu temple situated in Srivaikuntam town of Tamilnadu. Sri Kailasanathar Temple is dedicated to Lord Shiva. This is the 6th Nava Kailasam temple which is dedicated to Planet Saturn. The temple is originally believed to be built by the Pandiya king, Chandrakula Pandiya. He built the central shrine and vimana of the temple. Veerappa Nayak (1609-23 AD), a ruler of Madurai Nayak dynasty built the Yagasala, flag staff and Sandana Sababathy hall.According to the legend, Sage Romasa wanted to install the Shivalingas on the banks of the Thamirabarani. So, he asked his guru Agasthiya about this, who advised to throw flowers used for Shiva puja on the river and do the installations wherever the flowers reached the shores. Based on his advice, sage Romasa threw lotus flowers, nine of these flowers reached the bank. One lotus flower reached Srivaikuntam and is dedicated to one of the planets Sri Sani Bhagawan.The temple was constructed in the Dravidian style of architecture. It has three precincts. Shiva is worshipped as Kailasanathar and his consort Parvati as Sivakami. Sri Sani Bhagawan Sannidhi is situated separately. Those who are affected by Sani dosha pray to Sri Kailasanathar and Sri Sani to get the curse relieved. It is a belief that this is equal to Thirunallaru Sani Bhagawan temple. A guardian deity, ... ... Overview Sri Kailasanathar Temple - Srivaikuntam Tourist Places</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="2" t="inlineStr">
-        <is>
-          <t>Papanasam Ramalingeswara Temple</t>
-        </is>
-      </c>
-      <c r="B32" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 15 km from Kumbakonam, Ramalingaswara Temple is a Hindu temple located at Papanasam in the Thanjavur district of Tamil Nadu, India. Located near the south bank of the Kudamurutti river, it is one of the prominent places to visit as part of Kumbakonam Pilgrimage Tour.Papanasam Ramalingaswara Temple is a sacred temple dedicated to Lord Shiva, featuring a total of 108 Shiva Lingas. According to mythology, after defeating Ravana, Rama performed the brahmahathi dosha nivaranam puja at Rameswaram. In addition, he sought to appease Lord Shiva to atone for the sins incurred from the slaying of Kara and Dooshana, leading him to halt at this location. Here, he established 107 lingams and instructed Hanuman to retrieve one Lingam from Kasi to complete the total of 108. Consequently, the principal lingam is referred to as Ramalingaswami, while the one brought by Hanuman is known as Hanumanta Lingam. This site is also recognized as East Rameswaram or Keezh Rameswaram.The term Papanasam translates to 'Destruction of Sins' in Tamil, and it is widely believed that worshipping Lord Shiva at this temple absolves devotees of their sins. The main deity, Lord Ramalingaswami, resides in the central shrine. Within the hall, there are 106 Shiva Lingas arranged in three rows. Notably, the shrine is oriented towards the west, which deviates from traditional Hindu temple architectural guidelines, and ... ... Overview Papanasam Ramalingeswara Temple Tourist Places</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="inlineStr">
-        <is>
-          <t>Sri Vadivazhagiya Nambi Perumal Temple / Sundararaja Perumal Temple</t>
-        </is>
-      </c>
-      <c r="B33" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 34 km from Srirangam Railway Station, and 41 km from Trichy, Vadivazhagiya Nambi Perumal Temple, also known as Sundararaja Perumal Temple is a HIndu temple situated at Anbil village in the outskirts of Tiruchirappalli in Tamilnadu. It is one of the best places to visit near Trichy, and among the must-visit tourist places in Srirangam tour .Also known as Thiru Anbil, Vadivazhagiya Nambi Perumal Temple is dedicated to Lord Vishnu. It is one of the 108 Divya Desams of Lord Vishnu, who is worshipped here as Sundararajan and his consort as Sundaravalli. The temple is mentioned in the Naalayira Divya Prabandham, the ancient Tamil canon of the Alvar saints from the 6th-9th centuries CE.Located on the northern bank of the river Kollidam, the temple is believed to have been constructed by the Medieval Cholas of the late 8th century CE, with later contributions from Vijayanagara kings and Madurai Nayaks. Inscriptions on copper plates found in Anbil reveal the generous support provided by the Chola kings to this temple. Presently, the temple is maintained and overseen by the Hindu Religious and Endowment Board of the Government of Tamil Nadu.According to legend, the Hindu god of creation Brahma believed that he was the most handsome individual in the world as he created all the human beings. Upon learning this, Lord Vishnu cursed Brahma to be born as an earthly being. Brahma worshiped Vishnu for ... ... Overview Sri Vadivazhagiya Nambi Perumal Temple / Sundararaja Perumal Temple Tourist Places</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="2" t="inlineStr">
-        <is>
-          <t>Eri Katha Ramar Temple - Madhuranthakam</t>
-        </is>
-      </c>
-      <c r="B34" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage At a distance of 43 km from Mahabalipuram, Eri Katha Ramar Temple is a Hindu temple located in the town of Maduranthakam, Tamil Nadu, India. It is one of the most popular places to visit as part of Mahabalipuram pilgrimage packages.Sri Eri Katha Temple is dedicated to Lord Rama, revered here as Ramanujar. Constructed during the Pallava period, the temple is approximately 1600 years old, making it one of the oldest Rama temples in South India. The temple features inscriptions that attest to the generous donations made by Chola king Parantaka I. This site gained prominence during the Chola dynasty, known as Maduranthaga Chaturvedi Mangalam, named after the Chola ruler Madurantaga Uttama Chola (973-985 CE). The temple is also referred to by various names, including Vaikunda Varthanam, Thirumathurai, Thirumanthira Tirupathi, and Karunagara Vilagam.The temple is renowned for its association with the legend of Lord Rama safeguarding the Madurantakam Lake from flooding during intense rainfall. It is honored by figures such as Ramanujar and Thirumalisai Alvar and is recognized as one of the 108 Abhimana Kshethrams within the Vaishnavite tradition. This location is significant as it is where the presiding deity was named Ramanuja, and Thirumalisai Alvar achieved enlightenment here. Additionally, Sri Ramanujar received the Pancha Samskara Mantram at this site.The temple is constructed in the ... ... Overview Eri Katha Ramar Temple - Madhuranthakam Tourist Places</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="2" t="inlineStr">
-        <is>
-          <t>Rangaswamy Peak &amp; Pillar</t>
-        </is>
-      </c>
-      <c r="B35" s="2" t="inlineStr">
-        <is>
-          <t>Pilgrimage | Adventure / Trekking At a distance of 25 km from Kotagiri, Rangaswamy Peak is a famous mountain in the Eastern Ghats of Tamil Nadu near Kotagiri. It is one of the best places for trekking in Ooty Adventure packages.Rangaswamy Peak stands at an elevation of approximately 5,885 feet (1,794 meters). The peak is enveloped by a verdant landscape and features a temple dedicated to Lord Rangaswamy, making it a revered location for the Irula, Badaga, and Kurumba tribes of The Nilgiris. The devotees are allowed to visit the temple for only one month in the Tamil year (Puratasi).The Rangaswamy Peak Trek offers a stunning visual experience, showcasing the breathtaking beauty of nature and is considered one of the most exhilarating treks in Kotagiri. A scenic drive from Kotagiri to Kil (lower) Kotagiri via Kodanad Road leads to the trek's starting point, from which adventurers can embark on their journey to Rangaswamy Peak. The 5 km trek is moderately challenging, featuring a path of stone steps that wind through the vibrant tea estates. From this vantage point, trekkers can relish a magnificent view of the surrounding scenery, including dense forests, valleys, and nearby mountains.To the northwest of the peak, one can observe the impressive Rangaswamy Pillar, and is named in honor of Colonel J.C. Rangaswami, a European explorer who uncovered this remarkable site. The 400-foot-tall pillar is revered by the locals. The picturesque view of the shimmering waters of Upper Bhavani Reservoir, ... ... Overview Rangaswamy Peak &amp; Pillar Tourist Places No Destinations found for the selected filters Please wait... the destinations are being loaded Load more Top 6 Tamilnadu Tour Packages Package Duration Starting Price Details Hogenakkal - Yercaud 3D/2N ₹ 9050 View Details Kanchipuram - Mahabalipuram - Pondicherry 4D/3N ₹ 10750 View Details Madurai - Kanyakumari - Rameshwaram - Thanjavur 4D/3N ₹ 11350 View Details Chidambaram - Thanjavaur - Madurai - Rameshwaram - Trichy 5D/4N ₹ 14700 View Details Thanjavur - Madurai - Rameswaram - Trichy - Mahabalipuram 6D/5N ₹ 16850 View Details Best of Tamilnadu in 8 Days 8D/7N ₹ 22750 View Details All Tamilnadu Tour Packages Most Popular Tours Most Popular Tourist Places in Tamilnadu Ooty Tourist PlacesMadurai Tourist PlacesKodaikanal Tourist PlacesSrirangam Tourist PlacesRameshwaram Tourist PlacesTiruchirappalli Tourist PlacesYercaud Tourist PlacesKanyakumari Tourist PlacesCoonoor Tourist PlacesChidambaram Tourist PlacesChennai Tourist PlacesKanchipuram Tourist Places Popular Tour Packages in Tamilnadu Ooty Tour PackagesMadurai Tour PackagesKodaikanal Tour PackagesSrirangam Tour PackagesRameshwaram Tour PackagesTiruchirappalli Tour PackagesYercaud Tour PackagesKanyakumari Tour PackagesCoonoor Tour PackagesChidambaram Tour PackagesChennai Tour PackagesKanchipuram Tour Packages Popular Tour Packages near Chennai Mahabalipuram Tour PackagesKanchipuram Tour PackagesPondicherry Tour PackagesVellore Tour PackagesTirupati Tour PackagesKanipakam Tour PackagesSrikalahasti Tour PackagesYelagiri Hills Tour Packages 43 Best Pilgrimage Sites near Chennai 69 Best 2 Day Trips from Bangalore 74 Best 3 Day Trips from Bangalore 54 Best 2 Day Trips from Hyderabad 61 Best 3 Day Trips from Hyderabad 37 Best 2 Day Trips from Chennai 41 Best 3 Day Trips from Chennai 33 Best 2 Day Trips from Mumbai 20 Best 3 Day Trips from Mumbai 31 Best 2 Day Trips from Pune 18 Best 3 Day Trips from Pune 21 Best 2 Day Trips from Delhi 18 Best 3 Day Trips from Delhi 17 Best 2 Day Trips from Kochi 18 Best 3 Day Trips from Kochi 9 Best Goa Tour Packages Packages from Bangalore Packages from Hydearbad Packages from Chennai Packages from Mumbai Packages from Pune Packages from Delhi Packages from Kochi Similar GetawaysPilgrimage Sites in IndiaKarnataka Pilgrimage SitesTamilnadu Pilgrimage SitesKerala Pilgrimage SitesMaharashtra Pilgrimage SitesHimachal Pilgrimage SitesUttarakhand Pilgrimage SitesGoa Pilgrimage SitesRajasthan Pilgrimage SitesGujarat Pilgrimage SitesUttar Pradesh Pilgrimage SitesMadhya Pradesh Pilgrimage Sites Popular Chennai Getaways Top Places to Visit near Chennai Best Hill Stations around Chennai Best Waterfalls near Chennai Adventure / Trekking near Chennai Popular Beaches around Chennai Top Heritage Sites near Chennai Wildlife Sanctuaries near Chennai Pilgrimage Sites around Chennai Tamilnadu Tour PackagesPopular Tamilnadu GetawaysBest Places to Visit in TamilnaduTop Hill Stations in TamilnaduBest Waterfalls in TamilnaduBest Beaches in TamilnaduAdvanture / Trekking Sites in TamilnaduBest Pilgrimage Sites in TamilnaduHistorical / Heritage Sites in TamilnaduWildlife Parks in Tamilnadu Explore Tour Packages Destinations Getaways Cabs Hotels Blog Themes Honeymoon Hill Stations Wildlife Pilgrimage Beach Heritage Adventure Top Packages Coorg Packages Ooty Packages Goa Packages Shimla Packages Pondicherry Packages Mahabaleshwar Packages Chikmagalur Packages International Sri Lanka Thailand Bali Dubai Singapore Malaysia Maldives(Discontinued) 100% SECURE PAYMENTS Domestic &amp; International Cards Accepted Hotels Flights</t>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Annamalaiyar Temple, Thiruvannamalai</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>We conclude our list with another most significant Pancha Bhoota Sthala that signifies the element Agni. The temple is located on the foot of Annamalai hills and dates back to the 9th century of the Chola Dynasty. It is built in Dravidian style architecture and showcases the brilliant skills of artisans of that time. While the temple is usually crowded with tourists and locals, the footfall increases during the annual 'Karthigai Deepam Festival'. Devotees celebrate the festival wearing vibrant attires, and their huge possession comprises drummers and dancers.</t>
         </is>
       </c>
     </row>

</xml_diff>